<commit_message>
added new download button
</commit_message>
<xml_diff>
--- a/app/outputs/partner-solver-all-sheets.xlsx
+++ b/app/outputs/partner-solver-all-sheets.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3134" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3134" uniqueCount="240">
   <si>
     <t>Org</t>
   </si>
@@ -727,7 +727,16 @@
     <t>None</t>
   </si>
   <si>
-    <t>test area</t>
+    <t>None,AIR-INK: Air-Pollution to ink</t>
+  </si>
+  <si>
+    <t>None,Renewal Workshop</t>
+  </si>
+  <si>
+    <t>this is it!</t>
+  </si>
+  <si>
+    <t>Maybe not</t>
   </si>
 </sst>
 </file>
@@ -3264,13 +3273,13 @@
         <v>18</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -28158,13 +28167,13 @@
         <v>128</v>
       </c>
       <c r="B27" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -28312,13 +28321,13 @@
         <v>139</v>
       </c>
       <c r="B38" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:4">

</xml_diff>

<commit_message>
added ability to track all partners for solvers
</commit_message>
<xml_diff>
--- a/app/outputs/partner-solver-all-sheets.xlsx
+++ b/app/outputs/partner-solver-all-sheets.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Solver Team Data" sheetId="1" r:id="rId1"/>
     <sheet name="Partner Data" sheetId="2" r:id="rId2"/>
     <sheet name="Partner Solver Weights" sheetId="3" r:id="rId3"/>
+    <sheet name="Partner Match" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11914" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12152" uniqueCount="521">
   <si>
     <t>Challenge</t>
   </si>
@@ -1562,6 +1563,24 @@
   <si>
     <t>tech_weights</t>
   </si>
+  <si>
+    <t>Partners</t>
+  </si>
+  <si>
+    <t>Solvers</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>None,AHSA Platform</t>
+  </si>
 </sst>
 </file>
 
@@ -94961,4 +94980,1123 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D79"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" t="s">
+        <v>519</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" t="s">
+        <v>519</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" t="s">
+        <v>519</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" t="s">
+        <v>519</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6" t="s">
+        <v>519</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" t="s">
+        <v>519</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8" t="s">
+        <v>519</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B9" t="s">
+        <v>519</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B10" t="s">
+        <v>519</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" t="s">
+        <v>519</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B12" t="s">
+        <v>519</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" t="s">
+        <v>519</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B14" t="s">
+        <v>519</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B15" t="s">
+        <v>519</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>241</v>
+      </c>
+      <c r="B16" t="s">
+        <v>519</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>242</v>
+      </c>
+      <c r="B17" t="s">
+        <v>519</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>243</v>
+      </c>
+      <c r="B18" t="s">
+        <v>519</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>244</v>
+      </c>
+      <c r="B19" t="s">
+        <v>519</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>245</v>
+      </c>
+      <c r="B20" t="s">
+        <v>519</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>246</v>
+      </c>
+      <c r="B21" t="s">
+        <v>519</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" t="s">
+        <v>519</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>248</v>
+      </c>
+      <c r="B23" t="s">
+        <v>519</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>249</v>
+      </c>
+      <c r="B24" t="s">
+        <v>519</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>250</v>
+      </c>
+      <c r="B25" t="s">
+        <v>519</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>251</v>
+      </c>
+      <c r="B26" t="s">
+        <v>519</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>252</v>
+      </c>
+      <c r="B27" t="s">
+        <v>519</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>253</v>
+      </c>
+      <c r="B28" t="s">
+        <v>519</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>254</v>
+      </c>
+      <c r="B29" t="s">
+        <v>519</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>255</v>
+      </c>
+      <c r="B30" t="s">
+        <v>519</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>256</v>
+      </c>
+      <c r="B31" t="s">
+        <v>519</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>257</v>
+      </c>
+      <c r="B32" t="s">
+        <v>519</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>258</v>
+      </c>
+      <c r="B33" t="s">
+        <v>519</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>259</v>
+      </c>
+      <c r="B34" t="s">
+        <v>519</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>260</v>
+      </c>
+      <c r="B35" t="s">
+        <v>519</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>261</v>
+      </c>
+      <c r="B36" t="s">
+        <v>519</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>262</v>
+      </c>
+      <c r="B37" t="s">
+        <v>519</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>263</v>
+      </c>
+      <c r="B38" t="s">
+        <v>520</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>264</v>
+      </c>
+      <c r="B39" t="s">
+        <v>519</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>265</v>
+      </c>
+      <c r="B40" t="s">
+        <v>519</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>266</v>
+      </c>
+      <c r="B41" t="s">
+        <v>519</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>267</v>
+      </c>
+      <c r="B42" t="s">
+        <v>519</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>268</v>
+      </c>
+      <c r="B43" t="s">
+        <v>519</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>269</v>
+      </c>
+      <c r="B44" t="s">
+        <v>519</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>270</v>
+      </c>
+      <c r="B45" t="s">
+        <v>519</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>271</v>
+      </c>
+      <c r="B46" t="s">
+        <v>519</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>272</v>
+      </c>
+      <c r="B47" t="s">
+        <v>519</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>273</v>
+      </c>
+      <c r="B48" t="s">
+        <v>519</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>274</v>
+      </c>
+      <c r="B49" t="s">
+        <v>519</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>275</v>
+      </c>
+      <c r="B50" t="s">
+        <v>519</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>276</v>
+      </c>
+      <c r="B51" t="s">
+        <v>519</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>277</v>
+      </c>
+      <c r="B52" t="s">
+        <v>519</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>278</v>
+      </c>
+      <c r="B53" t="s">
+        <v>519</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>279</v>
+      </c>
+      <c r="B54" t="s">
+        <v>519</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>280</v>
+      </c>
+      <c r="B55" t="s">
+        <v>519</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>281</v>
+      </c>
+      <c r="B56" t="s">
+        <v>519</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>282</v>
+      </c>
+      <c r="B57" t="s">
+        <v>519</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>283</v>
+      </c>
+      <c r="B58" t="s">
+        <v>519</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>284</v>
+      </c>
+      <c r="B59" t="s">
+        <v>519</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>285</v>
+      </c>
+      <c r="B60" t="s">
+        <v>519</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>286</v>
+      </c>
+      <c r="B61" t="s">
+        <v>519</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>287</v>
+      </c>
+      <c r="B62" t="s">
+        <v>519</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>288</v>
+      </c>
+      <c r="B63" t="s">
+        <v>519</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>289</v>
+      </c>
+      <c r="B64" t="s">
+        <v>519</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>290</v>
+      </c>
+      <c r="B65" t="s">
+        <v>519</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>291</v>
+      </c>
+      <c r="B66" t="s">
+        <v>519</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>292</v>
+      </c>
+      <c r="B67" t="s">
+        <v>519</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>293</v>
+      </c>
+      <c r="B68" t="s">
+        <v>519</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>294</v>
+      </c>
+      <c r="B69" t="s">
+        <v>520</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>295</v>
+      </c>
+      <c r="B70" t="s">
+        <v>519</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>296</v>
+      </c>
+      <c r="B71" t="s">
+        <v>519</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>297</v>
+      </c>
+      <c r="B72" t="s">
+        <v>519</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>298</v>
+      </c>
+      <c r="B73" t="s">
+        <v>519</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>299</v>
+      </c>
+      <c r="B74" t="s">
+        <v>519</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>300</v>
+      </c>
+      <c r="B75" t="s">
+        <v>519</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>301</v>
+      </c>
+      <c r="B76" t="s">
+        <v>520</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>302</v>
+      </c>
+      <c r="B77" t="s">
+        <v>519</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>303</v>
+      </c>
+      <c r="B78" t="s">
+        <v>519</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>304</v>
+      </c>
+      <c r="B79" t="s">
+        <v>519</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79" t="s">
+        <v>519</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>